<commit_message>
correcting the confidence intervals
</commit_message>
<xml_diff>
--- a/data/df_after_pca.xlsx
+++ b/data/df_after_pca.xlsx
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>0.00184060371801951</v>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -1504,7 +1504,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>0.1394196013632139</v>
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0.8535132989281461</v>
@@ -1928,7 +1928,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>4.905089870653452</v>
@@ -2034,7 +2034,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
         <v>2.732608486481285</v>
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
         <v>0.9258806859823131</v>
@@ -2246,7 +2246,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="n">
         <v>0.9528851244044468</v>
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -2670,7 +2670,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -2776,7 +2776,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
         <v>0.8999133227961047</v>
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
         <v>2.605039974727224</v>
@@ -2988,7 +2988,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
         <v>0.124155740961462</v>
@@ -3200,7 +3200,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -3306,7 +3306,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -3412,7 +3412,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -3518,7 +3518,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
         <v>0.5757052389176741</v>
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" t="n">
         <v>0.1748408499955169</v>
@@ -3836,7 +3836,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="n">
         <v>0.0691426313709996</v>
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -4154,7 +4154,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -4260,7 +4260,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -4472,7 +4472,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
         <v>0.04926108374384236</v>
@@ -4578,7 +4578,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40" t="n">
         <v>0.1899783400491282</v>
@@ -4684,7 +4684,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -4790,7 +4790,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -5108,7 +5108,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -5320,7 +5320,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -5638,7 +5638,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -5850,7 +5850,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -5956,7 +5956,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -6168,7 +6168,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
         <v>0.005725190839694656</v>
@@ -6486,7 +6486,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58" t="n">
         <v>0.2158828064764842</v>
@@ -6698,7 +6698,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60" t="n">
         <v>0.04204183162246435</v>
@@ -6804,7 +6804,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61" t="n">
         <v>0.5195914445353927</v>
@@ -6910,7 +6910,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
@@ -7016,7 +7016,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" t="n">
         <v>0.00436109899694723</v>
@@ -7228,7 +7228,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
@@ -7440,7 +7440,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -7652,7 +7652,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -7758,7 +7758,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
@@ -7864,7 +7864,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
@@ -8079,7 +8079,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -8167,7 +8167,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -8255,7 +8255,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -8431,7 +8431,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -8519,7 +8519,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -8607,7 +8607,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -8695,7 +8695,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -8783,7 +8783,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -8871,7 +8871,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
         <v>0.1762</v>
@@ -9223,7 +9223,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -9399,7 +9399,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -9487,7 +9487,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -9575,7 +9575,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -9663,7 +9663,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -9751,7 +9751,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -9927,7 +9927,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -10015,7 +10015,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
         <v>3.5846</v>
@@ -10103,7 +10103,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -10279,7 +10279,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -10543,7 +10543,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -10631,7 +10631,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -10719,7 +10719,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -10895,7 +10895,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -10983,7 +10983,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="n">
         <v>2.0539</v>
@@ -11071,7 +11071,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -11335,7 +11335,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -11511,7 +11511,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -11687,7 +11687,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -11863,7 +11863,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -11951,7 +11951,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" t="n">
         <v>3.7401</v>
@@ -12039,7 +12039,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -12215,7 +12215,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -12303,7 +12303,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -12391,7 +12391,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -12479,7 +12479,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -12567,7 +12567,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -12655,7 +12655,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C54" t="n">
         <v>0.0154</v>
@@ -12743,7 +12743,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
@@ -12919,7 +12919,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -13271,7 +13271,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
@@ -13359,7 +13359,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
@@ -13447,7 +13447,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
@@ -13535,7 +13535,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
@@ -13623,7 +13623,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
@@ -13711,7 +13711,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
@@ -13799,7 +13799,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -13887,7 +13887,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
@@ -13975,7 +13975,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -14063,7 +14063,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
@@ -14151,7 +14151,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Revisiting MIC from Colab
</commit_message>
<xml_diff>
--- a/data/df_after_pca.xlsx
+++ b/data/df_after_pca.xlsx
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -868,7 +868,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
         <v>0.00184060371801951</v>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -1504,7 +1504,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
         <v>0.8535132989281461</v>
@@ -1928,7 +1928,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
         <v>4.905089870653452</v>
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>0.9258806859823131</v>
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
         <v>2.605039974727224</v>
@@ -3200,7 +3200,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -3518,7 +3518,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
         <v>0.5757052389176741</v>
@@ -3730,7 +3730,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -4048,7 +4048,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35" t="n">
         <v>0.55</v>
@@ -4154,7 +4154,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -4260,7 +4260,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -4578,7 +4578,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
         <v>0.1899783400491282</v>
@@ -4790,7 +4790,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -5002,7 +5002,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="n">
         <v>0.1675206937327552</v>
@@ -5320,7 +5320,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -5638,7 +5638,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -5744,7 +5744,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -5850,7 +5850,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -6168,7 +6168,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55" t="n">
         <v>0.005725190839694656</v>
@@ -6274,7 +6274,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" t="n">
         <v>0.003489305279318887</v>
@@ -6486,7 +6486,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" t="n">
         <v>0.2158828064764842</v>
@@ -6592,7 +6592,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
@@ -6698,7 +6698,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" t="n">
         <v>0.04204183162246435</v>
@@ -6804,7 +6804,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" t="n">
         <v>0.5195914445353927</v>
@@ -7016,7 +7016,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" t="n">
         <v>0.00436109899694723</v>
@@ -7122,7 +7122,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
@@ -7228,7 +7228,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
@@ -7334,7 +7334,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
         <v>0.2721829069134458</v>
@@ -7440,7 +7440,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -7758,7 +7758,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
@@ -8079,7 +8079,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -8255,7 +8255,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -8343,7 +8343,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -8431,7 +8431,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -8519,7 +8519,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -8607,7 +8607,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -8695,7 +8695,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -8783,7 +8783,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -8959,7 +8959,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -9223,7 +9223,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -9311,7 +9311,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -9399,7 +9399,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -9751,7 +9751,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -10103,7 +10103,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -10279,7 +10279,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -10367,7 +10367,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -10631,7 +10631,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -10719,7 +10719,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -10895,7 +10895,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -11247,7 +11247,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -11335,7 +11335,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -11423,7 +11423,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -11511,7 +11511,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -11599,7 +11599,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -11863,7 +11863,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -12039,7 +12039,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -12127,7 +12127,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -12215,7 +12215,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -12303,7 +12303,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -12391,7 +12391,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -12831,7 +12831,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C56" t="n">
         <v>0.007</v>
@@ -13095,7 +13095,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
@@ -13183,7 +13183,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
@@ -13359,7 +13359,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
@@ -13447,7 +13447,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
@@ -13535,7 +13535,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
@@ -13623,7 +13623,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
@@ -13711,7 +13711,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
@@ -13887,7 +13887,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
@@ -14063,7 +14063,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>

</xml_diff>